<commit_message>
[#1389] Add layer to check if sheets is empty
</commit_message>
<xml_diff>
--- a/backend/api/v1/v1_profile/tests/fixtures/entities-test-2.xlsx
+++ b/backend/api/v1/v1_profile/tests/fixtures/entities-test-2.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="School" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Health Care Facilities" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -191,7 +192,7 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -283,4 +284,27 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>